<commit_message>
remove column from alcohol data
</commit_message>
<xml_diff>
--- a/resource/alcohol/13.05.16/1/measurement-1.xlsx
+++ b/resource/alcohol/13.05.16/1/measurement-1.xlsx
@@ -61,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,16 +158,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P10" activeCellId="0" sqref="P10"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,9 +207,6 @@
         <v>0</v>
       </c>
       <c r="M1" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -247,9 +244,6 @@
       <c r="M2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -283,9 +277,6 @@
         <v>-1</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -323,9 +314,6 @@
       <c r="M4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
@@ -359,9 +347,6 @@
         <v>1</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="N5" s="2" t="n">
         <v>20</v>
       </c>
     </row>
@@ -397,9 +382,6 @@
         <v>4</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>48</v>
-      </c>
-      <c r="N6" s="2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -435,9 +417,6 @@
         <v>6</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N7" s="2" t="n">
         <v>19</v>
       </c>
     </row>
@@ -473,9 +452,6 @@
         <v>7</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N8" s="2" t="n">
         <v>19</v>
       </c>
     </row>
@@ -507,9 +483,6 @@
         <v>7</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N9" s="2" t="n">
         <v>20</v>
       </c>
     </row>
@@ -541,9 +514,6 @@
         <v>8</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N10" s="2" t="n">
         <v>19</v>
       </c>
     </row>
@@ -575,9 +545,6 @@
         <v>8</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N11" s="2" t="n">
         <v>20</v>
       </c>
     </row>
@@ -609,9 +576,6 @@
         <v>8</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N12" s="2" t="n">
         <v>21</v>
       </c>
     </row>
@@ -643,9 +607,6 @@
         <v>9</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N13" s="2" t="n">
         <v>21</v>
       </c>
     </row>
@@ -677,9 +638,6 @@
         <v>8</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N14" s="2" t="n">
         <v>21</v>
       </c>
     </row>
@@ -711,9 +669,6 @@
         <v>9</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N15" s="2" t="n">
         <v>21</v>
       </c>
     </row>
@@ -745,9 +700,6 @@
         <v>9</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N16" s="2" t="n">
         <v>21</v>
       </c>
     </row>
@@ -779,9 +731,6 @@
         <v>9</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N17" s="2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -813,9 +762,6 @@
         <v>10</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N18" s="2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -847,9 +793,6 @@
         <v>9</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N19" s="2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -881,9 +824,6 @@
         <v>10</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N20" s="2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -915,9 +855,6 @@
         <v>10</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N21" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -949,9 +886,6 @@
         <v>11</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N22" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -983,9 +917,6 @@
         <v>10</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N23" s="2" t="n">
         <v>22</v>
       </c>
     </row>
@@ -1017,9 +948,6 @@
         <v>10</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N24" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1051,9 +979,6 @@
         <v>11</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N25" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1085,9 +1010,6 @@
         <v>11</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N26" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1119,9 +1041,6 @@
         <v>11</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N27" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1153,9 +1072,6 @@
         <v>11</v>
       </c>
       <c r="M28" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N28" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1187,9 +1103,6 @@
         <v>11</v>
       </c>
       <c r="M29" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N29" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1221,9 +1134,6 @@
         <v>11</v>
       </c>
       <c r="M30" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N30" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1255,9 +1165,6 @@
         <v>11</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N31" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1289,9 +1196,6 @@
         <v>11</v>
       </c>
       <c r="M32" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N32" s="2" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1323,9 +1227,6 @@
         <v>12</v>
       </c>
       <c r="M33" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N33" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1357,9 +1258,6 @@
         <v>11</v>
       </c>
       <c r="M34" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N34" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1391,9 +1289,6 @@
         <v>12</v>
       </c>
       <c r="M35" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N35" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1425,9 +1320,6 @@
         <v>11</v>
       </c>
       <c r="M36" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N36" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1459,9 +1351,6 @@
         <v>12</v>
       </c>
       <c r="M37" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N37" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1493,9 +1382,6 @@
         <v>12</v>
       </c>
       <c r="M38" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N38" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1527,9 +1413,6 @@
         <v>11</v>
       </c>
       <c r="M39" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N39" s="2" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1561,9 +1444,6 @@
         <v>11</v>
       </c>
       <c r="M40" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N40" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1595,9 +1475,6 @@
         <v>12</v>
       </c>
       <c r="M41" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N41" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1629,9 +1506,6 @@
         <v>12</v>
       </c>
       <c r="M42" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N42" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1663,9 +1537,6 @@
         <v>12</v>
       </c>
       <c r="M43" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N43" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1697,9 +1568,6 @@
         <v>12</v>
       </c>
       <c r="M44" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N44" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1731,9 +1599,6 @@
         <v>11</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N45" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1765,9 +1630,6 @@
         <v>12</v>
       </c>
       <c r="M46" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N46" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1799,9 +1661,6 @@
         <v>12</v>
       </c>
       <c r="M47" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N47" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1833,9 +1692,6 @@
         <v>13</v>
       </c>
       <c r="M48" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N48" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1867,9 +1723,6 @@
         <v>12</v>
       </c>
       <c r="M49" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N49" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1901,9 +1754,6 @@
         <v>13</v>
       </c>
       <c r="M50" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N50" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1935,9 +1785,6 @@
         <v>13</v>
       </c>
       <c r="M51" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N51" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1969,9 +1816,6 @@
         <v>12</v>
       </c>
       <c r="M52" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N52" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2003,9 +1847,6 @@
         <v>12</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N53" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -2037,9 +1878,6 @@
         <v>13</v>
       </c>
       <c r="M54" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N54" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2071,9 +1909,6 @@
         <v>13</v>
       </c>
       <c r="M55" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N55" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -2105,9 +1940,6 @@
         <v>13</v>
       </c>
       <c r="M56" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N56" s="2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -2139,9 +1971,6 @@
         <v>13</v>
       </c>
       <c r="M57" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N57" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2173,9 +2002,6 @@
         <v>13</v>
       </c>
       <c r="M58" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N58" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2207,9 +2033,6 @@
         <v>13</v>
       </c>
       <c r="M59" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N59" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2241,9 +2064,6 @@
         <v>13</v>
       </c>
       <c r="M60" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N60" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2275,9 +2095,6 @@
         <v>13</v>
       </c>
       <c r="M61" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N61" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2309,9 +2126,6 @@
         <v>13</v>
       </c>
       <c r="M62" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N62" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2343,9 +2157,6 @@
         <v>14</v>
       </c>
       <c r="M63" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N63" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2377,9 +2188,6 @@
         <v>13</v>
       </c>
       <c r="M64" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N64" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2411,9 +2219,6 @@
         <v>13</v>
       </c>
       <c r="M65" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N65" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2445,9 +2250,6 @@
         <v>13</v>
       </c>
       <c r="M66" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N66" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2479,9 +2281,6 @@
         <v>14</v>
       </c>
       <c r="M67" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="N67" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2513,9 +2312,6 @@
         <v>13</v>
       </c>
       <c r="M68" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N68" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2547,9 +2343,6 @@
         <v>13</v>
       </c>
       <c r="M69" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N69" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2581,9 +2374,6 @@
         <v>14</v>
       </c>
       <c r="M70" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N70" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2615,9 +2405,6 @@
         <v>14</v>
       </c>
       <c r="M71" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N71" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2649,9 +2436,6 @@
         <v>14</v>
       </c>
       <c r="M72" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N72" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2683,9 +2467,6 @@
         <v>14</v>
       </c>
       <c r="M73" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N73" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2717,9 +2498,6 @@
         <v>14</v>
       </c>
       <c r="M74" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N74" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2751,9 +2529,6 @@
         <v>14</v>
       </c>
       <c r="M75" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N75" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2785,9 +2560,6 @@
         <v>14</v>
       </c>
       <c r="M76" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N76" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2819,9 +2591,6 @@
         <v>14</v>
       </c>
       <c r="M77" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N77" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2853,9 +2622,6 @@
         <v>14</v>
       </c>
       <c r="M78" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N78" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2887,9 +2653,6 @@
         <v>14</v>
       </c>
       <c r="M79" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N79" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2921,9 +2684,6 @@
         <v>14</v>
       </c>
       <c r="M80" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N80" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2955,9 +2715,6 @@
         <v>14</v>
       </c>
       <c r="M81" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N81" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2989,9 +2746,6 @@
         <v>14</v>
       </c>
       <c r="M82" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N82" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3023,9 +2777,6 @@
         <v>14</v>
       </c>
       <c r="M83" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N83" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3057,9 +2808,6 @@
         <v>15</v>
       </c>
       <c r="M84" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N84" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3091,9 +2839,6 @@
         <v>14</v>
       </c>
       <c r="M85" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="N85" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3125,9 +2870,6 @@
         <v>15</v>
       </c>
       <c r="M86" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N86" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3159,9 +2901,6 @@
         <v>14</v>
       </c>
       <c r="M87" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N87" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3193,9 +2932,6 @@
         <v>14</v>
       </c>
       <c r="M88" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N88" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3227,9 +2963,6 @@
         <v>15</v>
       </c>
       <c r="M89" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N89" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3261,9 +2994,6 @@
         <v>15</v>
       </c>
       <c r="M90" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N90" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3295,9 +3025,6 @@
         <v>14</v>
       </c>
       <c r="M91" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N91" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3329,9 +3056,6 @@
         <v>14</v>
       </c>
       <c r="M92" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N92" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3363,9 +3087,6 @@
         <v>15</v>
       </c>
       <c r="M93" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N93" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3397,9 +3118,6 @@
         <v>15</v>
       </c>
       <c r="M94" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N94" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3431,9 +3149,6 @@
         <v>14</v>
       </c>
       <c r="M95" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N95" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3465,9 +3180,6 @@
         <v>14</v>
       </c>
       <c r="M96" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N96" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3499,9 +3211,6 @@
         <v>14</v>
       </c>
       <c r="M97" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N97" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3533,9 +3242,6 @@
         <v>15</v>
       </c>
       <c r="M98" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N98" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3567,9 +3273,6 @@
         <v>15</v>
       </c>
       <c r="M99" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N99" s="2" t="n">
         <v>28</v>
       </c>
     </row>
@@ -3601,9 +3304,6 @@
         <v>15</v>
       </c>
       <c r="M100" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N100" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3635,9 +3335,6 @@
         <v>15</v>
       </c>
       <c r="M101" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N101" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3669,9 +3366,6 @@
         <v>15</v>
       </c>
       <c r="M102" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N102" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3703,9 +3397,6 @@
         <v>14</v>
       </c>
       <c r="M103" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N103" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3737,9 +3428,6 @@
         <v>15</v>
       </c>
       <c r="M104" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N104" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3771,9 +3459,6 @@
         <v>15</v>
       </c>
       <c r="M105" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N105" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3805,9 +3490,6 @@
         <v>15</v>
       </c>
       <c r="M106" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N106" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3839,9 +3521,6 @@
         <v>15</v>
       </c>
       <c r="M107" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="N107" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3873,9 +3552,6 @@
         <v>15</v>
       </c>
       <c r="M108" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N108" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -3907,9 +3583,6 @@
         <v>15</v>
       </c>
       <c r="M109" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N109" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3941,9 +3614,6 @@
         <v>16</v>
       </c>
       <c r="M110" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N110" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3975,9 +3645,6 @@
         <v>15</v>
       </c>
       <c r="M111" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N111" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4009,9 +3676,6 @@
         <v>15</v>
       </c>
       <c r="M112" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N112" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4043,9 +3707,6 @@
         <v>16</v>
       </c>
       <c r="M113" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N113" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4077,9 +3738,6 @@
         <v>15</v>
       </c>
       <c r="M114" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N114" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4111,9 +3769,6 @@
         <v>15</v>
       </c>
       <c r="M115" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N115" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4145,9 +3800,6 @@
         <v>16</v>
       </c>
       <c r="M116" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N116" s="2" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4179,9 +3831,6 @@
         <v>16</v>
       </c>
       <c r="M117" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N117" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4213,9 +3862,6 @@
         <v>16</v>
       </c>
       <c r="M118" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="N118" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4247,9 +3893,6 @@
         <v>16</v>
       </c>
       <c r="M119" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="N119" s="2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4271,21 +3914,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -4300,21 +3942,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>